<commit_message>
excel to object array/about us section/configured excwl/cross browser testing code updated
</commit_message>
<xml_diff>
--- a/OpenEMRApplication/TestData/OpenEMRData.xlsx
+++ b/OpenEMRApplication/TestData/OpenEMRData.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sollers\Azure Full Stack June 2021\SDET Track\SeleniumWebdriverConcept\OpenEMRApplication\OpenEMRApplication\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B592F14-AAF8-4820-8763-2542DC795D9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{567AE60D-AEEC-4D72-8BAE-EBC181414872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InvalidCredentialTest" sheetId="1" r:id="rId1"/>
+    <sheet name="AddPatientTest" sheetId="2" r:id="rId2"/>
+    <sheet name="VersionNumberTest" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
-  <si>
-    <t>usename</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
   <si>
     <t xml:space="preserve">language </t>
   </si>
@@ -42,9 +41,6 @@
     <t>Invalid username or password</t>
   </si>
   <si>
-    <t>Dutch</t>
-  </si>
-  <si>
     <t>John</t>
   </si>
   <si>
@@ -55,6 +51,66 @@
   </si>
   <si>
     <t>Peter123</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>English (Standard)</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>fName</t>
+  </si>
+  <si>
+    <t>lName</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>ExpectedPatientName</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>2021-07-19</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>expectedVersion</t>
+  </si>
+  <si>
+    <t>Version Number: v6.0.0 (1)</t>
+  </si>
+  <si>
+    <t>Medical Record Dashboard - John Smith</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>2021-07-21</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Medical Record Dashboard - Jack Jack</t>
   </si>
 </sst>
 </file>
@@ -90,8 +146,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,55 +431,203 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99AA4F21-E8F7-4200-BF22-64D840657031}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="17.21875" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="1"/>
+    <col min="8" max="8" width="38.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C889A40-BE7E-4C19-ABD1-92D3F95C1CB2}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
+      <c r="D2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>